<commit_message>
Revert "Revert "Update Team Planning""
This reverts commit f25fda53f521489eb3095ccb8aca585cbf216ea4.
</commit_message>
<xml_diff>
--- a/Phase 2-Team Planning_W23_.xlsx
+++ b/Phase 2-Team Planning_W23_.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YZN\Desktop\uOttawa_Teaching\CSI4142\Project\Physical Design_Data Staging\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\uOttawa\CSI\4142\CSI4142_Group15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8973AB91-80AA-45BD-9727-6CFE35290847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7555B60E-148F-46AE-B253-A4D3CEF0464E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BC7B5491-6718-42D3-AD60-469765C6A1D2}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BC7B5491-6718-42D3-AD60-469765C6A1D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
   <si>
     <t>Deliverable checklist</t>
   </si>
@@ -68,18 +57,6 @@
     <t xml:space="preserve">Create database instance </t>
   </si>
   <si>
-    <t xml:space="preserve">Create &lt;name&gt; dimension </t>
-  </si>
-  <si>
-    <t>Create &lt;name&gt; dimension</t>
-  </si>
-  <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t>Staging of dimension &lt;name&gt;</t>
-  </si>
-  <si>
     <t>Surrogate key pipeline</t>
   </si>
   <si>
@@ -89,9 +66,6 @@
     <t xml:space="preserve">Data quality handling and reporting </t>
   </si>
   <si>
-    <t>Others – if any</t>
-  </si>
-  <si>
     <t>Phase 2- Physical design and data staging</t>
   </si>
   <si>
@@ -99,6 +73,69 @@
   </si>
   <si>
     <t>CSI4142 - Project W23</t>
+  </si>
+  <si>
+    <t>Zhiyuan Lin</t>
+  </si>
+  <si>
+    <t>Lixiong Wei</t>
+  </si>
+  <si>
+    <t>1 hour</t>
+  </si>
+  <si>
+    <t>1 day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 day </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Date dimension </t>
+  </si>
+  <si>
+    <t>Create Province dimension</t>
+  </si>
+  <si>
+    <t>Create vaccination dimension</t>
+  </si>
+  <si>
+    <t>Create COVID19Metric dimension</t>
+  </si>
+  <si>
+    <t>Staging of dimension Date</t>
+  </si>
+  <si>
+    <t>Staging of dimension Province</t>
+  </si>
+  <si>
+    <t>Staging of dimension Vaccination</t>
+  </si>
+  <si>
+    <t>Staging of dimension COVID19 Metric</t>
+  </si>
+  <si>
+    <t>SQL statement design</t>
+  </si>
+  <si>
+    <t>2 hour</t>
+  </si>
+  <si>
+    <t>3 hour</t>
+  </si>
+  <si>
+    <t>0.5 day</t>
+  </si>
+  <si>
+    <t>3 hours</t>
+  </si>
+  <si>
+    <t>6 hours</t>
+  </si>
+  <si>
+    <t>8 hour</t>
+  </si>
+  <si>
+    <t>create a connection between python and postgre</t>
   </si>
 </sst>
 </file>
@@ -190,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -204,6 +241,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -214,6 +255,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -530,41 +574,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825036BF-4FD7-4D21-BD38-801A4B8E13C8}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="28" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="28" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="9" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -573,168 +617,341 @@
       <c r="F6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="8"/>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="5">
+        <v>45366</v>
+      </c>
+      <c r="D8" s="5">
+        <v>45368</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="5">
+        <v>45367</v>
+      </c>
+      <c r="D9" s="5">
+        <v>45370</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="5">
+        <v>45367</v>
+      </c>
+      <c r="D10" s="5">
+        <v>45370</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="5">
+        <v>45367</v>
+      </c>
+      <c r="D11" s="5">
+        <v>45370</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="5">
+        <v>45367</v>
+      </c>
+      <c r="D12" s="5">
+        <v>45370</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="5">
+        <v>45366</v>
+      </c>
+      <c r="D13" s="5">
+        <v>45368</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="5">
+        <v>45368</v>
+      </c>
+      <c r="D14" s="5">
+        <v>45369</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="5">
+        <v>45368</v>
+      </c>
+      <c r="D15" s="5">
+        <v>45369</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="5">
+        <v>45368</v>
+      </c>
+      <c r="D16" s="5">
+        <v>45369</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="5">
+        <v>45368</v>
+      </c>
+      <c r="D17" s="5">
+        <v>45369</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="B18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="6">
+        <v>45370</v>
+      </c>
+      <c r="D18" s="5">
+        <v>45370</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="B19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="5">
+        <v>45371</v>
+      </c>
+      <c r="D19" s="5">
+        <v>45371</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+      <c r="B20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="5">
+        <v>45371</v>
+      </c>
+      <c r="D20" s="5">
+        <v>45370</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
+      <c r="C21" s="11">
+        <v>45369</v>
+      </c>
+      <c r="D21" s="11">
+        <v>45370</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="G21:G22"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="G6:G7"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>